<commit_message>
Added Decimal Places column
</commit_message>
<xml_diff>
--- a/Docs/FieldValidationTemplate.xlsx
+++ b/Docs/FieldValidationTemplate.xlsx
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Field Name</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>json</t>
+  </si>
+  <si>
+    <t>Decimal Places</t>
   </si>
 </sst>
 </file>
@@ -293,8 +296,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P1048576" totalsRowShown="0">
-  <autoFilter ref="A1:P1048576">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q1048576" totalsRowShown="0">
+  <autoFilter ref="A1:Q1048576">
     <filterColumn colId="2"/>
     <filterColumn colId="5"/>
     <filterColumn colId="6"/>
@@ -302,8 +305,9 @@
     <filterColumn colId="11"/>
     <filterColumn colId="12"/>
     <filterColumn colId="13"/>
+    <filterColumn colId="14"/>
   </autoFilter>
-  <tableColumns count="16">
+  <tableColumns count="17">
     <tableColumn id="1" name="Field Name"/>
     <tableColumn id="2" name="Field Label"/>
     <tableColumn id="10" name="Parent Field Name"/>
@@ -316,6 +320,7 @@
     <tableColumn id="6" name="Required?"/>
     <tableColumn id="15" name="Min "/>
     <tableColumn id="14" name="Max "/>
+    <tableColumn id="11" name="Decimal Places"/>
     <tableColumn id="16" name="Regex Pattern"/>
     <tableColumn id="17" name="Format"/>
     <tableColumn id="7" name="Error Message"/>
@@ -610,11 +615,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P2000"/>
+  <dimension ref="A1:Q2000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -627,13 +632,13 @@
     <col min="7" max="7" width="21.140625" customWidth="1"/>
     <col min="8" max="8" width="28.28515625" customWidth="1"/>
     <col min="9" max="9" width="30.42578125" customWidth="1"/>
-    <col min="10" max="14" width="12.140625" customWidth="1"/>
-    <col min="15" max="15" width="28.42578125" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" customWidth="1"/>
-    <col min="32" max="33" width="9.140625" customWidth="1"/>
+    <col min="10" max="15" width="12.140625" customWidth="1"/>
+    <col min="16" max="16" width="28.42578125" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" customWidth="1"/>
+    <col min="33" max="34" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -671,15 +676,18 @@
         <v>30</v>
       </c>
       <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added data type longtext for textarea instead of text
</commit_message>
<xml_diff>
--- a/Docs/FieldValidationTemplate.xlsx
+++ b/Docs/FieldValidationTemplate.xlsx
@@ -33,7 +33,7 @@
     <definedName name="signature">Sheet2!$D$7</definedName>
     <definedName name="survey">Sheet2!$D$8</definedName>
     <definedName name="tags">Sheet2!$D$6</definedName>
-    <definedName name="textarea">Sheet2!$D$5</definedName>
+    <definedName name="textarea">Sheet2!$D$10</definedName>
     <definedName name="textfield">Sheet2!$D$5</definedName>
     <definedName name="time">Sheet2!$D$9:$E$9</definedName>
     <definedName name="url">Sheet2!$D$5</definedName>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Field Name</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>Decimal Places</t>
+  </si>
+  <si>
+    <t>longtext</t>
   </si>
 </sst>
 </file>
@@ -725,9 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -815,6 +816,9 @@
     <row r="10" spans="2:5">
       <c r="B10" t="s">
         <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:5">

</xml_diff>